<commit_message>
updating basestation eeprom documentation
</commit_message>
<xml_diff>
--- a/Wireless/LORD MicroStrain Wireless Configuration.xlsx
+++ b/Wireless/LORD MicroStrain Wireless Configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wireless Node Config" sheetId="3" r:id="rId1"/>
@@ -2685,9 +2685,6 @@
     <t>The minimum wake interval is internally limited to 1 second (a value of 7680), and the maximum wake interval is limited to approximately 15 seconds (a value of 512). Any values outside of this range will be automatically truncated.</t>
   </si>
   <si>
-    <t>LORD MicroStrain Base Station EEPROM Map  -  10/19/2015</t>
-  </si>
-  <si>
     <t>Calibration Coefficients</t>
   </si>
   <si>
@@ -3049,9 +3046,6 @@
   </si>
   <si>
     <t>Acceleration threshold for inactivity in G's</t>
-  </si>
-  <si>
-    <t>LORD MicroStrain Wireless Node EEPROM Map  -  10/23/2015</t>
   </si>
   <si>
     <t>Bootloader</t>
@@ -3204,10 +3198,16 @@
     <t>0 for standard angle mode, 1 for distributed angle mode, 2 for raw gauge strain mode.</t>
   </si>
   <si>
-    <t>Whether the beacon is echoed over the port (2) or not (0).</t>
-  </si>
-  <si>
-    <t>[0, 2]</t>
+    <t>[0-3]</t>
+  </si>
+  <si>
+    <t>Controls beacon echos over the port (0 = off, 1 = echo rx, 2 = echo tx, 3 = echo both)</t>
+  </si>
+  <si>
+    <t>LORD MicroStrain Base Station EEPROM Map  -  12/03/2015</t>
+  </si>
+  <si>
+    <t>LORD MicroStrain Wireless Node EEPROM Map  -  12/03/2015</t>
   </si>
 </sst>
 </file>
@@ -3806,12 +3806,6 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3847,6 +3841,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4643,7 +4643,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C264" sqref="C264"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4657,39 +4657,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
-        <v>841</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="A1" s="76" t="s">
+        <v>889</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="80" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="76" t="s">
-        <v>779</v>
+      <c r="H2" s="74" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4699,12 +4699,12 @@
       <c r="B3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="77"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="75"/>
     </row>
     <row r="4" spans="1:8" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -4728,7 +4728,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4753,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4778,7 +4778,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4801,7 +4801,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4824,7 +4824,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4847,7 +4847,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4874,7 +4874,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4901,7 +4901,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4926,7 +4926,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4953,7 +4953,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4970,7 +4970,7 @@
       <c r="D14" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="74"/>
+      <c r="E14" s="86"/>
       <c r="F14" s="70" t="s">
         <v>8</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="64" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="C15" s="71"/>
       <c r="D15" s="69"/>
-      <c r="E15" s="75"/>
+      <c r="E15" s="87"/>
       <c r="F15" s="71"/>
       <c r="G15" s="73"/>
       <c r="H15" s="65"/>
@@ -5020,7 +5020,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5045,7 +5045,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5095,7 +5095,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5120,7 +5120,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5172,7 +5172,7 @@
         <v>7</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5199,7 +5199,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5226,7 +5226,7 @@
         <v>7</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5251,7 +5251,7 @@
         <v>7</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5276,7 +5276,7 @@
         <v>8</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5301,7 +5301,7 @@
         <v>8</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5328,7 +5328,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5380,7 +5380,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5407,7 +5407,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5434,7 +5434,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5457,7 +5457,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5484,7 +5484,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5511,7 +5511,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5534,7 +5534,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5561,7 +5561,7 @@
         <v>1</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5586,7 +5586,7 @@
         <v>7</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5613,7 +5613,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5640,7 +5640,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5667,7 +5667,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5694,7 +5694,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5721,7 +5721,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5748,7 +5748,7 @@
         <v>4</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5775,7 +5775,7 @@
         <v>4</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5800,7 +5800,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5825,7 +5825,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5850,7 +5850,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5875,7 +5875,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5902,7 +5902,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5927,7 +5927,7 @@
         <v>3</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5952,7 +5952,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -5977,7 +5977,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6002,7 +6002,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6027,7 +6027,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6052,7 +6052,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6077,7 +6077,7 @@
         <v>1</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6104,7 +6104,7 @@
         <v>1</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6129,7 +6129,7 @@
         <v>1</v>
       </c>
       <c r="H59" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6169,7 +6169,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6211,7 +6211,7 @@
         <v>1</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6236,7 +6236,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6276,7 +6276,7 @@
         <v>1</v>
       </c>
       <c r="H66" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6318,7 +6318,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6343,7 +6343,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6383,7 +6383,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6425,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6450,7 +6450,7 @@
         <v>1</v>
       </c>
       <c r="H74" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6490,7 +6490,7 @@
         <v>1</v>
       </c>
       <c r="H76" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6532,7 +6532,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6557,7 +6557,7 @@
         <v>1</v>
       </c>
       <c r="H79" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6597,7 +6597,7 @@
         <v>1</v>
       </c>
       <c r="H81" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6664,7 +6664,7 @@
         <v>1</v>
       </c>
       <c r="H84" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6704,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6746,7 +6746,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6771,7 +6771,7 @@
         <v>1</v>
       </c>
       <c r="H89" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6811,7 +6811,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6853,7 +6853,7 @@
         <v>1</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6878,7 +6878,7 @@
         <v>1</v>
       </c>
       <c r="H94" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6918,7 +6918,7 @@
         <v>1</v>
       </c>
       <c r="H96" s="64" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6945,7 +6945,7 @@
         <v>0xE6</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>10</v>
@@ -6958,7 +6958,7 @@
         <v>1</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6970,7 +6970,7 @@
         <v>0xE8</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>10</v>
@@ -6983,7 +6983,7 @@
         <v>1</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -6995,7 +6995,7 @@
         <v>0xEA</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>10</v>
@@ -7008,7 +7008,7 @@
         <v>1</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7020,7 +7020,7 @@
         <v>0xEC</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>10</v>
@@ -7033,7 +7033,7 @@
         <v>1</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7045,7 +7045,7 @@
         <v>0xEE</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>10</v>
@@ -7058,7 +7058,7 @@
         <v>1</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7070,7 +7070,7 @@
         <v>0xF0</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>10</v>
@@ -7083,7 +7083,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7095,7 +7095,7 @@
         <v>0xF6</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>10</v>
@@ -7108,7 +7108,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="104.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -7133,7 +7133,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7151,16 +7151,16 @@
         <v>10</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G106" s="9">
         <v>1</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7185,7 +7185,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7210,7 +7210,7 @@
         <v>1</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7235,7 +7235,7 @@
         <v>1</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7262,7 +7262,7 @@
         <v>7</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7287,7 +7287,7 @@
         <v>7</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7312,7 +7312,7 @@
         <v>7</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7337,7 +7337,7 @@
         <v>7</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7362,7 +7362,7 @@
         <v>7</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7389,7 +7389,7 @@
         <v>7</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7414,7 +7414,7 @@
         <v>7</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7439,7 +7439,7 @@
         <v>7</v>
       </c>
       <c r="H117" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7464,7 +7464,7 @@
         <v>7</v>
       </c>
       <c r="H118" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7491,7 +7491,7 @@
         <v>8</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7516,7 +7516,7 @@
         <v>1</v>
       </c>
       <c r="H120" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7541,7 +7541,7 @@
         <v>1</v>
       </c>
       <c r="H121" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7566,7 +7566,7 @@
         <v>1</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7591,7 +7591,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7616,7 +7616,7 @@
         <v>1</v>
       </c>
       <c r="H124" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7641,7 +7641,7 @@
         <v>1</v>
       </c>
       <c r="H125" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7666,7 +7666,7 @@
         <v>1</v>
       </c>
       <c r="H126" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7691,7 +7691,7 @@
         <v>1</v>
       </c>
       <c r="H127" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7716,7 +7716,7 @@
         <v>1</v>
       </c>
       <c r="H128" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7741,7 +7741,7 @@
         <v>1</v>
       </c>
       <c r="H129" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7766,7 +7766,7 @@
         <v>1</v>
       </c>
       <c r="H130" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7791,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="H131" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7816,7 +7816,7 @@
         <v>1</v>
       </c>
       <c r="H132" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7841,7 +7841,7 @@
         <v>1</v>
       </c>
       <c r="H133" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7866,7 +7866,7 @@
         <v>1</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7891,7 +7891,7 @@
         <v>1</v>
       </c>
       <c r="H135" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7916,7 +7916,7 @@
         <v>1</v>
       </c>
       <c r="H136" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7941,7 +7941,7 @@
         <v>1</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7966,7 +7966,7 @@
         <v>1</v>
       </c>
       <c r="H138" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -7991,7 +7991,7 @@
         <v>1</v>
       </c>
       <c r="H139" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8016,7 +8016,7 @@
         <v>1</v>
       </c>
       <c r="H140" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8041,7 +8041,7 @@
         <v>1</v>
       </c>
       <c r="H141" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8066,7 +8066,7 @@
         <v>1</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8091,7 +8091,7 @@
         <v>1</v>
       </c>
       <c r="H143" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8116,7 +8116,7 @@
         <v>1</v>
       </c>
       <c r="H144" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8141,7 +8141,7 @@
         <v>1</v>
       </c>
       <c r="H145" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8166,7 +8166,7 @@
         <v>1</v>
       </c>
       <c r="H146" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8191,7 +8191,7 @@
         <v>1</v>
       </c>
       <c r="H147" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8216,7 +8216,7 @@
         <v>1</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8241,7 +8241,7 @@
         <v>1</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8266,7 +8266,7 @@
         <v>1</v>
       </c>
       <c r="H150" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8291,7 +8291,7 @@
         <v>1</v>
       </c>
       <c r="H151" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="152" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8316,7 +8316,7 @@
         <v>1</v>
       </c>
       <c r="H152" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8341,7 +8341,7 @@
         <v>1</v>
       </c>
       <c r="H153" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8366,7 +8366,7 @@
         <v>1</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8391,7 +8391,7 @@
         <v>1</v>
       </c>
       <c r="H155" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8416,7 +8416,7 @@
         <v>1</v>
       </c>
       <c r="H156" s="5" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8441,7 +8441,7 @@
         <v>1</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8466,7 +8466,7 @@
         <v>1</v>
       </c>
       <c r="H158" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="159" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8506,7 +8506,7 @@
         <v>1</v>
       </c>
       <c r="H160" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8546,7 +8546,7 @@
         <v>1</v>
       </c>
       <c r="H162" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8586,7 +8586,7 @@
         <v>1</v>
       </c>
       <c r="H164" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8626,7 +8626,7 @@
         <v>1</v>
       </c>
       <c r="H166" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8666,7 +8666,7 @@
         <v>1</v>
       </c>
       <c r="H168" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8706,7 +8706,7 @@
         <v>1</v>
       </c>
       <c r="H170" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8746,7 +8746,7 @@
         <v>1</v>
       </c>
       <c r="H172" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="173" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8786,7 +8786,7 @@
         <v>1</v>
       </c>
       <c r="H174" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="175" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8826,7 +8826,7 @@
         <v>1</v>
       </c>
       <c r="H176" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8866,7 +8866,7 @@
         <v>1</v>
       </c>
       <c r="H178" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8906,7 +8906,7 @@
         <v>1</v>
       </c>
       <c r="H180" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="181" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8946,7 +8946,7 @@
         <v>1</v>
       </c>
       <c r="H182" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -8986,7 +8986,7 @@
         <v>1</v>
       </c>
       <c r="H184" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9026,7 +9026,7 @@
         <v>1</v>
       </c>
       <c r="H186" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9066,7 +9066,7 @@
         <v>1</v>
       </c>
       <c r="H188" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9106,7 +9106,7 @@
         <v>1</v>
       </c>
       <c r="H190" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="191" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9146,7 +9146,7 @@
         <v>1</v>
       </c>
       <c r="H192" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9186,7 +9186,7 @@
         <v>1</v>
       </c>
       <c r="H194" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9226,7 +9226,7 @@
         <v>1</v>
       </c>
       <c r="H196" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="197" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9266,7 +9266,7 @@
         <v>1</v>
       </c>
       <c r="H198" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="199" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9306,7 +9306,7 @@
         <v>1</v>
       </c>
       <c r="H200" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9346,7 +9346,7 @@
         <v>1</v>
       </c>
       <c r="H202" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="203" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9386,7 +9386,7 @@
         <v>1</v>
       </c>
       <c r="H204" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="205" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9426,7 +9426,7 @@
         <v>1</v>
       </c>
       <c r="H206" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="207" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9466,7 +9466,7 @@
         <v>1</v>
       </c>
       <c r="H208" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9506,7 +9506,7 @@
         <v>1</v>
       </c>
       <c r="H210" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="211" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9546,7 +9546,7 @@
         <v>1</v>
       </c>
       <c r="H212" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="213" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9586,7 +9586,7 @@
         <v>1</v>
       </c>
       <c r="H214" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="215" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9626,7 +9626,7 @@
         <v>1</v>
       </c>
       <c r="H216" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="217" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9666,7 +9666,7 @@
         <v>1</v>
       </c>
       <c r="H218" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="219" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9706,7 +9706,7 @@
         <v>1</v>
       </c>
       <c r="H220" s="64" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="221" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9748,7 +9748,7 @@
         <v>1</v>
       </c>
       <c r="H222" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="223" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9775,7 +9775,7 @@
         <v>1</v>
       </c>
       <c r="H223" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="224" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9802,7 +9802,7 @@
         <v>1</v>
       </c>
       <c r="H224" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="225" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9814,20 +9814,20 @@
         <v>0x2AA</v>
       </c>
       <c r="C225" s="44" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D225" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E225" s="45"/>
       <c r="F225" s="46" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G225" s="47">
         <v>7</v>
       </c>
       <c r="H225" s="43" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="226" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9839,22 +9839,22 @@
         <v>0x2AC</v>
       </c>
       <c r="C226" s="6" t="s">
+        <v>788</v>
+      </c>
+      <c r="D226" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E226" s="7">
+        <v>1</v>
+      </c>
+      <c r="F226" s="8" t="s">
         <v>789</v>
-      </c>
-      <c r="D226" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E226" s="7">
-        <v>1</v>
-      </c>
-      <c r="F226" s="8" t="s">
-        <v>790</v>
       </c>
       <c r="G226" s="9">
         <v>7</v>
       </c>
       <c r="H226" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="227" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9866,20 +9866,20 @@
         <v>0x2AE</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D227" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E227" s="7"/>
       <c r="F227" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G227" s="9">
         <v>7</v>
       </c>
       <c r="H227" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9891,20 +9891,20 @@
         <v>0x2B0</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D228" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E228" s="7"/>
       <c r="F228" s="8" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G228" s="9">
         <v>7</v>
       </c>
       <c r="H228" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9916,20 +9916,20 @@
         <v>0x2BC</v>
       </c>
       <c r="C229" s="66" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D229" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E229" s="68"/>
       <c r="F229" s="70" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G229" s="72">
         <v>7</v>
       </c>
       <c r="H229" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="230" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9956,20 +9956,20 @@
         <v>0x2C0</v>
       </c>
       <c r="C231" s="66" t="s">
+        <v>812</v>
+      </c>
+      <c r="D231" s="68" t="s">
         <v>813</v>
-      </c>
-      <c r="D231" s="68" t="s">
-        <v>814</v>
       </c>
       <c r="E231" s="68"/>
       <c r="F231" s="70" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G231" s="72">
         <v>7</v>
       </c>
       <c r="H231" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="232" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -9996,20 +9996,20 @@
         <v>0x2C4</v>
       </c>
       <c r="C233" s="66" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D233" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E233" s="68"/>
       <c r="F233" s="70" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G233" s="72">
         <v>7</v>
       </c>
       <c r="H233" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="234" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10036,20 +10036,20 @@
         <v>0x2C8</v>
       </c>
       <c r="C235" s="66" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D235" s="68" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E235" s="68"/>
       <c r="F235" s="70" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="G235" s="72">
         <v>7</v>
       </c>
       <c r="H235" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="236" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10076,20 +10076,20 @@
         <v>0x2CC</v>
       </c>
       <c r="C237" s="66" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D237" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E237" s="68"/>
       <c r="F237" s="70" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G237" s="72">
         <v>10</v>
       </c>
       <c r="H237" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="238" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10116,20 +10116,20 @@
         <v>0x2D0</v>
       </c>
       <c r="C239" s="66" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D239" s="68" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E239" s="68"/>
       <c r="F239" s="70" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="G239" s="72">
         <v>10</v>
       </c>
       <c r="H239" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="240" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10156,20 +10156,20 @@
         <v>0x2D4</v>
       </c>
       <c r="C241" s="66" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D241" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E241" s="68"/>
       <c r="F241" s="70" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G241" s="72">
         <v>10</v>
       </c>
       <c r="H241" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="242" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10196,20 +10196,20 @@
         <v>0x2D8</v>
       </c>
       <c r="C243" s="66" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D243" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E243" s="68"/>
       <c r="F243" s="70" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G243" s="72">
         <v>10</v>
       </c>
       <c r="H243" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10236,20 +10236,20 @@
         <v>0x2DC</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D245" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E245" s="7"/>
       <c r="F245" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="G245" s="9">
         <v>10</v>
       </c>
       <c r="H245" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="246" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10261,20 +10261,20 @@
         <v>0x2DE</v>
       </c>
       <c r="C246" s="66" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D246" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E246" s="68"/>
       <c r="F246" s="70" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G246" s="72">
         <v>7</v>
       </c>
       <c r="H246" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10301,20 +10301,20 @@
         <v>0x2E2</v>
       </c>
       <c r="C248" s="66" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D248" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E248" s="68"/>
       <c r="F248" s="70" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G248" s="72">
         <v>7</v>
       </c>
       <c r="H248" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10341,20 +10341,20 @@
         <v>0x2E6</v>
       </c>
       <c r="C250" s="66" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D250" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E250" s="68"/>
       <c r="F250" s="70" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G250" s="72">
         <v>7</v>
       </c>
       <c r="H250" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="251" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10381,22 +10381,22 @@
         <v>0x2EA</v>
       </c>
       <c r="C252" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="D252" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E252" s="7" t="s">
+        <v>884</v>
+      </c>
+      <c r="F252" s="8" t="s">
         <v>885</v>
       </c>
-      <c r="D252" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E252" s="7" t="s">
-        <v>886</v>
-      </c>
-      <c r="F252" s="8" t="s">
-        <v>887</v>
-      </c>
       <c r="G252" s="9">
         <v>10</v>
       </c>
       <c r="H252" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="253" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10408,22 +10408,22 @@
         <v>0x2EC</v>
       </c>
       <c r="C253" s="6" t="s">
+        <v>797</v>
+      </c>
+      <c r="D253" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E253" s="7" t="s">
         <v>798</v>
       </c>
-      <c r="D253" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E253" s="7" t="s">
+      <c r="F253" s="8" t="s">
         <v>799</v>
       </c>
-      <c r="F253" s="8" t="s">
-        <v>800</v>
-      </c>
       <c r="G253" s="9">
         <v>10</v>
       </c>
       <c r="H253" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="254" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10435,20 +10435,20 @@
         <v>0x2EE</v>
       </c>
       <c r="C254" s="66" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D254" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E254" s="68"/>
       <c r="F254" s="70" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G254" s="72">
         <v>10</v>
       </c>
       <c r="H254" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="255" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10475,20 +10475,20 @@
         <v>0x2F2</v>
       </c>
       <c r="C256" s="66" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D256" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E256" s="68"/>
       <c r="F256" s="70" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G256" s="72">
         <v>10</v>
       </c>
       <c r="H256" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="257" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10515,20 +10515,20 @@
         <v>0x30E</v>
       </c>
       <c r="C258" s="66" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D258" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E258" s="68"/>
       <c r="F258" s="70" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G258" s="72">
         <v>10</v>
       </c>
       <c r="H258" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="259" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10555,20 +10555,20 @@
         <v>0x312</v>
       </c>
       <c r="C260" s="66" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D260" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E260" s="68"/>
       <c r="F260" s="70" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G260" s="72">
         <v>10</v>
       </c>
       <c r="H260" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="261" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10595,20 +10595,20 @@
         <v>0x316</v>
       </c>
       <c r="C262" s="66" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D262" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E262" s="68"/>
       <c r="F262" s="70" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G262" s="72">
         <v>10</v>
       </c>
       <c r="H262" s="64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="263" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10635,22 +10635,22 @@
         <v>0x33A</v>
       </c>
       <c r="C264" s="6" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="D264" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E264" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F264" s="8" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="G264" s="9">
         <v>10</v>
       </c>
       <c r="H264" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="265" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10662,22 +10662,22 @@
         <v>0x342</v>
       </c>
       <c r="C265" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D265" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E265" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="F265" s="8" t="s">
         <v>830</v>
       </c>
-      <c r="D265" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E265" s="7" t="s">
-        <v>788</v>
-      </c>
-      <c r="F265" s="8" t="s">
-        <v>831</v>
-      </c>
       <c r="G265" s="9">
         <v>10</v>
       </c>
       <c r="H265" s="5" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="266" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10689,20 +10689,20 @@
         <v>0x344</v>
       </c>
       <c r="C266" s="66" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D266" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E266" s="68"/>
       <c r="F266" s="70" t="s">
+        <v>832</v>
+      </c>
+      <c r="G266" s="72">
+        <v>10</v>
+      </c>
+      <c r="H266" s="64" t="s">
         <v>833</v>
-      </c>
-      <c r="G266" s="72">
-        <v>10</v>
-      </c>
-      <c r="H266" s="64" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="267" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10729,20 +10729,20 @@
         <v>0x348</v>
       </c>
       <c r="C268" s="66" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D268" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E268" s="68"/>
       <c r="F268" s="70" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G268" s="72">
         <v>10</v>
       </c>
       <c r="H268" s="64" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="269" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10769,20 +10769,20 @@
         <v>0x34C</v>
       </c>
       <c r="C270" s="66" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D270" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E270" s="68"/>
       <c r="F270" s="70" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="G270" s="72">
         <v>10</v>
       </c>
       <c r="H270" s="64" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="271" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10809,20 +10809,20 @@
         <v>0x350</v>
       </c>
       <c r="C272" s="66" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D272" s="68" t="s">
         <v>52</v>
       </c>
       <c r="E272" s="68"/>
       <c r="F272" s="70" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G272" s="72">
         <v>10</v>
       </c>
       <c r="H272" s="64" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="273" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10849,22 +10849,22 @@
         <v>0x354</v>
       </c>
       <c r="C274" s="49" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D274" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E274" s="50" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F274" s="51" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="G274" s="52">
         <v>10</v>
       </c>
       <c r="H274" s="54" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="275" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10876,22 +10876,22 @@
         <v>0x406</v>
       </c>
       <c r="C275" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="D275" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E275" s="7" t="s">
         <v>843</v>
       </c>
-      <c r="D275" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E275" s="7" t="s">
-        <v>845</v>
-      </c>
       <c r="F275" s="8" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="G275" s="9">
         <v>10</v>
       </c>
       <c r="H275" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="276" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10903,7 +10903,7 @@
         <v>0x408</v>
       </c>
       <c r="C276" s="6" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D276" s="7" t="s">
         <v>10</v>
@@ -10912,13 +10912,13 @@
         <v>11</v>
       </c>
       <c r="F276" s="8" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="G276" s="9">
         <v>10</v>
       </c>
       <c r="H276" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="277" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10930,22 +10930,22 @@
         <v>0x40A</v>
       </c>
       <c r="C277" s="6" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D277" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E277" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F277" s="8" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="G277" s="9">
         <v>10</v>
       </c>
       <c r="H277" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="278" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10957,22 +10957,22 @@
         <v>0x40C</v>
       </c>
       <c r="C278" s="66" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D278" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E278" s="86" t="s">
-        <v>848</v>
+      <c r="E278" s="84" t="s">
+        <v>846</v>
       </c>
       <c r="F278" s="70" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="G278" s="72">
         <v>10</v>
       </c>
       <c r="H278" s="64" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="279" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -10985,7 +10985,7 @@
       </c>
       <c r="C279" s="67"/>
       <c r="D279" s="69"/>
-      <c r="E279" s="87"/>
+      <c r="E279" s="85"/>
       <c r="F279" s="71"/>
       <c r="G279" s="73"/>
       <c r="H279" s="65"/>
@@ -10999,22 +10999,22 @@
         <v>0x410</v>
       </c>
       <c r="C280" s="6" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D280" s="7" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="E280" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F280" s="8" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="G280" s="9">
         <v>10</v>
       </c>
       <c r="H280" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -11755,9 +11755,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -11773,39 +11773,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
-        <v>719</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="A1" s="76" t="s">
+        <v>888</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="80" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="76" t="s">
-        <v>779</v>
+      <c r="H2" s="74" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="3" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
@@ -11815,12 +11815,12 @@
       <c r="B3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="77"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="75"/>
     </row>
     <row r="4" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
@@ -11844,7 +11844,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="64" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -11877,16 +11877,16 @@
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="G6" s="9">
-        <v>1</v>
+        <v>3.34</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -11911,7 +11911,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -11936,7 +11936,7 @@
         <v>3</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -11963,7 +11963,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -11990,7 +11990,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12017,7 +12017,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12044,7 +12044,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12071,7 +12071,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12098,7 +12098,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12125,7 +12125,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12150,7 +12150,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12175,7 +12175,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12200,7 +12200,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12227,7 +12227,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12252,7 +12252,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12277,7 +12277,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12302,7 +12302,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12327,7 +12327,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12367,7 +12367,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12407,7 +12407,7 @@
         <v>3</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12432,7 +12432,7 @@
         <v>3</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12457,7 +12457,7 @@
         <v>3</v>
       </c>
       <c r="H29" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12497,7 +12497,7 @@
         <v>3</v>
       </c>
       <c r="H31" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12537,7 +12537,7 @@
         <v>3</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12562,7 +12562,7 @@
         <v>3</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12587,7 +12587,7 @@
         <v>3</v>
       </c>
       <c r="H35" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12627,7 +12627,7 @@
         <v>3</v>
       </c>
       <c r="H37" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12667,7 +12667,7 @@
         <v>3</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12692,7 +12692,7 @@
         <v>3</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12717,7 +12717,7 @@
         <v>3</v>
       </c>
       <c r="H41" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12757,7 +12757,7 @@
         <v>3</v>
       </c>
       <c r="H43" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12797,7 +12797,7 @@
         <v>3</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12822,7 +12822,7 @@
         <v>3</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12847,7 +12847,7 @@
         <v>3</v>
       </c>
       <c r="H47" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12887,7 +12887,7 @@
         <v>3</v>
       </c>
       <c r="H49" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12927,7 +12927,7 @@
         <v>3</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12952,7 +12952,7 @@
         <v>3</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -12977,7 +12977,7 @@
         <v>3</v>
       </c>
       <c r="H53" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13017,7 +13017,7 @@
         <v>3</v>
       </c>
       <c r="H55" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13057,7 +13057,7 @@
         <v>3</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13082,7 +13082,7 @@
         <v>3</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13107,7 +13107,7 @@
         <v>3</v>
       </c>
       <c r="H59" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13147,7 +13147,7 @@
         <v>3</v>
       </c>
       <c r="H61" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13187,7 +13187,7 @@
         <v>3</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13212,7 +13212,7 @@
         <v>3</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13237,7 +13237,7 @@
         <v>3</v>
       </c>
       <c r="H65" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13277,7 +13277,7 @@
         <v>3</v>
       </c>
       <c r="H67" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13319,7 +13319,7 @@
         <v>3</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13344,7 +13344,7 @@
         <v>3</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13371,7 +13371,7 @@
         <v>3</v>
       </c>
       <c r="H71" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13413,7 +13413,7 @@
         <v>3</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13438,7 +13438,7 @@
         <v>3</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13465,7 +13465,7 @@
         <v>3</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13490,7 +13490,7 @@
         <v>2.27</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13515,7 +13515,7 @@
         <v>1</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13533,16 +13533,16 @@
         <v>10</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G78" s="9">
         <v>1</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13567,7 +13567,7 @@
         <v>3</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13594,7 +13594,7 @@
         <v>3</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13619,7 +13619,7 @@
         <v>3</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13646,7 +13646,7 @@
         <v>3</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13671,7 +13671,7 @@
         <v>3</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13698,7 +13698,7 @@
         <v>3</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13723,7 +13723,7 @@
         <v>3</v>
       </c>
       <c r="H85" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13763,7 +13763,7 @@
         <v>3</v>
       </c>
       <c r="H87" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13805,7 +13805,7 @@
         <v>3</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13817,22 +13817,22 @@
         <v>0x406</v>
       </c>
       <c r="C90" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>843</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>845</v>
-      </c>
       <c r="F90" s="8" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="G90" s="9">
         <v>10</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13844,7 +13844,7 @@
         <v>0x408</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D91" s="7" t="s">
         <v>10</v>
@@ -13853,13 +13853,13 @@
         <v>11</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="G91" s="9">
         <v>10</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13871,22 +13871,22 @@
         <v>0x40A</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="G92" s="9">
         <v>10</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13898,22 +13898,22 @@
         <v>0x40C</v>
       </c>
       <c r="C93" s="66" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D93" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E93" s="86" t="s">
-        <v>848</v>
+      <c r="E93" s="84" t="s">
+        <v>846</v>
       </c>
       <c r="F93" s="70" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="G93" s="72">
         <v>10</v>
       </c>
       <c r="H93" s="64" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
@@ -13926,7 +13926,7 @@
       </c>
       <c r="C94" s="67"/>
       <c r="D94" s="69"/>
-      <c r="E94" s="87"/>
+      <c r="E94" s="85"/>
       <c r="F94" s="71"/>
       <c r="G94" s="73"/>
       <c r="H94" s="65"/>
@@ -13940,22 +13940,22 @@
         <v>0x410</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="G95" s="9">
         <v>10</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -14149,7 +14149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C407"/>
   <sheetViews>
-    <sheetView topLeftCell="A381" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A398" sqref="A398:C398"/>
     </sheetView>
   </sheetViews>
@@ -15377,13 +15377,13 @@
     </row>
     <row r="152" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="99" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B152" s="100"/>
     </row>
     <row r="153" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="101" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B153" s="102"/>
     </row>
@@ -16563,14 +16563,14 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="96" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B329" s="97"/>
       <c r="C329" s="98"/>
     </row>
     <row r="330" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="129" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B330" s="130"/>
       <c r="C330" s="131"/>
@@ -16582,7 +16582,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="132" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B332" s="133"/>
       <c r="C332" s="134"/>
@@ -16594,7 +16594,7 @@
     </row>
     <row r="334" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="112" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B334" s="113"/>
       <c r="C334" s="114"/>
@@ -16606,7 +16606,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="132" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B336" s="133"/>
       <c r="C336" s="134"/>
@@ -16622,25 +16622,25 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="24" t="s">
+        <v>724</v>
+      </c>
+      <c r="B338" s="17" t="s">
         <v>725</v>
-      </c>
-      <c r="B338" s="17" t="s">
-        <v>726</v>
       </c>
       <c r="C338" s="27"/>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="24" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B339" s="17" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C339" s="27"/>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="24" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B340" s="17" t="s">
         <v>52</v>
@@ -16649,7 +16649,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="24" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B341" s="17" t="s">
         <v>52</v>
@@ -16663,14 +16663,14 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="123" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B343" s="124"/>
       <c r="C343" s="125"/>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="118" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B344" s="119"/>
       <c r="C344" s="120"/>
@@ -16691,10 +16691,10 @@
         <v>0</v>
       </c>
       <c r="B346" s="41" t="s">
+        <v>731</v>
+      </c>
+      <c r="C346" s="27" t="s">
         <v>732</v>
-      </c>
-      <c r="C346" s="27" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -16702,10 +16702,10 @@
         <v>4</v>
       </c>
       <c r="B347" s="41" t="s">
+        <v>733</v>
+      </c>
+      <c r="C347" s="27" t="s">
         <v>734</v>
-      </c>
-      <c r="C347" s="27" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -16715,14 +16715,14 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="123" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B349" s="124"/>
       <c r="C349" s="125"/>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="118" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B350" s="119"/>
       <c r="C350" s="120"/>
@@ -16743,10 +16743,10 @@
         <v>0</v>
       </c>
       <c r="B352" s="17" t="s">
+        <v>737</v>
+      </c>
+      <c r="C352" s="27" t="s">
         <v>738</v>
-      </c>
-      <c r="C352" s="27" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
@@ -16754,10 +16754,10 @@
         <v>1</v>
       </c>
       <c r="B353" s="17" t="s">
+        <v>739</v>
+      </c>
+      <c r="C353" s="27" t="s">
         <v>740</v>
-      </c>
-      <c r="C353" s="27" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -16765,7 +16765,7 @@
         <v>2</v>
       </c>
       <c r="B354" s="17" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C354" s="27"/>
     </row>
@@ -16774,7 +16774,7 @@
         <v>3</v>
       </c>
       <c r="B355" s="17" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C355" s="27"/>
     </row>
@@ -16783,7 +16783,7 @@
         <v>4</v>
       </c>
       <c r="B356" s="17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C356" s="27"/>
     </row>
@@ -16792,7 +16792,7 @@
         <v>5</v>
       </c>
       <c r="B357" s="17" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C357" s="27"/>
     </row>
@@ -16801,7 +16801,7 @@
         <v>6</v>
       </c>
       <c r="B358" s="17" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C358" s="27"/>
     </row>
@@ -16810,7 +16810,7 @@
         <v>7</v>
       </c>
       <c r="B359" s="17" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C359" s="27"/>
     </row>
@@ -16819,7 +16819,7 @@
         <v>8</v>
       </c>
       <c r="B360" s="17" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C360" s="27"/>
     </row>
@@ -16828,7 +16828,7 @@
         <v>9</v>
       </c>
       <c r="B361" s="17" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C361" s="27"/>
     </row>
@@ -16837,7 +16837,7 @@
         <v>10</v>
       </c>
       <c r="B362" s="17" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C362" s="27"/>
     </row>
@@ -16846,7 +16846,7 @@
         <v>11</v>
       </c>
       <c r="B363" s="17" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C363" s="27"/>
     </row>
@@ -16855,7 +16855,7 @@
         <v>12</v>
       </c>
       <c r="B364" s="17" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C364" s="27"/>
     </row>
@@ -16864,7 +16864,7 @@
         <v>13</v>
       </c>
       <c r="B365" s="17" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C365" s="27"/>
     </row>
@@ -16873,7 +16873,7 @@
         <v>14</v>
       </c>
       <c r="B366" s="17" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C366" s="27"/>
     </row>
@@ -16882,7 +16882,7 @@
         <v>15</v>
       </c>
       <c r="B367" s="17" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C367" s="27"/>
     </row>
@@ -16891,7 +16891,7 @@
         <v>16</v>
       </c>
       <c r="B368" s="17" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C368" s="27"/>
     </row>
@@ -16900,7 +16900,7 @@
         <v>17</v>
       </c>
       <c r="B369" s="17" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C369" s="27"/>
     </row>
@@ -16909,7 +16909,7 @@
         <v>18</v>
       </c>
       <c r="B370" s="17" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C370" s="27"/>
     </row>
@@ -16918,7 +16918,7 @@
         <v>19</v>
       </c>
       <c r="B371" s="17" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C371" s="27"/>
     </row>
@@ -16927,7 +16927,7 @@
         <v>20</v>
       </c>
       <c r="B372" s="17" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C372" s="27"/>
     </row>
@@ -16936,7 +16936,7 @@
         <v>21</v>
       </c>
       <c r="B373" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C373" s="27"/>
     </row>
@@ -16945,7 +16945,7 @@
         <v>22</v>
       </c>
       <c r="B374" s="17" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C374" s="27"/>
     </row>
@@ -16954,7 +16954,7 @@
         <v>23</v>
       </c>
       <c r="B375" s="17" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C375" s="27"/>
     </row>
@@ -16963,7 +16963,7 @@
         <v>24</v>
       </c>
       <c r="B376" s="17" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C376" s="27"/>
     </row>
@@ -16972,7 +16972,7 @@
         <v>25</v>
       </c>
       <c r="B377" s="17" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C377" s="27"/>
     </row>
@@ -16981,7 +16981,7 @@
         <v>26</v>
       </c>
       <c r="B378" s="17" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C378" s="27"/>
     </row>
@@ -16990,7 +16990,7 @@
         <v>27</v>
       </c>
       <c r="B379" s="17" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C379" s="27"/>
     </row>
@@ -16999,7 +16999,7 @@
         <v>28</v>
       </c>
       <c r="B380" s="17" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C380" s="27"/>
     </row>
@@ -17008,7 +17008,7 @@
         <v>29</v>
       </c>
       <c r="B381" s="17" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C381" s="27"/>
     </row>
@@ -17017,7 +17017,7 @@
         <v>30</v>
       </c>
       <c r="B382" s="17" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C382" s="27"/>
     </row>
@@ -17026,7 +17026,7 @@
         <v>31</v>
       </c>
       <c r="B383" s="17" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C383" s="27"/>
     </row>
@@ -17035,7 +17035,7 @@
         <v>32</v>
       </c>
       <c r="B384" s="17" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C384" s="27"/>
     </row>
@@ -17044,7 +17044,7 @@
         <v>33</v>
       </c>
       <c r="B385" s="17" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C385" s="27"/>
     </row>
@@ -17053,34 +17053,34 @@
         <v>34</v>
       </c>
       <c r="B386" s="18" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C386" s="28"/>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="96" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B388" s="97"/>
       <c r="C388" s="98"/>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="118" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B389" s="119"/>
       <c r="C389" s="120"/>
     </row>
     <row r="390" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="112" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B390" s="113"/>
       <c r="C390" s="114"/>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="22" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B391" s="142" t="s">
         <v>4</v>
@@ -17089,37 +17089,37 @@
     </row>
     <row r="392" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="48" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B392" s="130" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C392" s="131"/>
     </row>
     <row r="393" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="48" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B393" s="130" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C393" s="131"/>
     </row>
     <row r="394" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="48" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B394" s="130" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="C394" s="131"/>
     </row>
     <row r="395" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="48" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B395" s="130" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C395" s="131"/>
     </row>
@@ -17130,49 +17130,49 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="96" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B398" s="97"/>
       <c r="C398" s="98"/>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="118" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B399" s="119"/>
       <c r="C399" s="120"/>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="118" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B400" s="119"/>
       <c r="C400" s="120"/>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="112" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B401" s="113"/>
       <c r="C401" s="114"/>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="112" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B402" s="113"/>
       <c r="C402" s="114"/>
     </row>
     <row r="403" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="112" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B403" s="113"/>
       <c r="C403" s="114"/>
     </row>
     <row r="404" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="112" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B404" s="113"/>
       <c r="C404" s="114"/>

</xml_diff>